<commit_message>
better text sizing on fig 2 go terms in silico
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-CC-in_silico_combined.xlsx
+++ b/analyses/unipept/GO-terms/GO-CC-in_silico_combined.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GO-CC-in_silico_combined" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="113">
   <si>
     <t xml:space="preserve">GO term</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t xml:space="preserve">Photosystem II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endoplasmic reticulum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golgi appartatus</t>
   </si>
 </sst>
 </file>
@@ -3056,10 +3062,10 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
+      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4777,14 +4783,366 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>227</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>213</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fig 2 condensed even more
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/GO-CC-in_silico_combined.xlsx
+++ b/analyses/unipept/GO-terms/GO-CC-in_silico_combined.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="111">
   <si>
     <t xml:space="preserve">GO term</t>
   </si>
@@ -356,12 +356,6 @@
   </si>
   <si>
     <t xml:space="preserve">Photosystem II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endoplasmic reticulum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golgi appartatus</t>
   </si>
 </sst>
 </file>
@@ -376,6 +370,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -397,6 +392,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -404,6 +400,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -558,7 +555,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.07"/>
@@ -1800,10 +1797,10 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3047,7 +3044,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3062,16 +3059,16 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -3579,35 +3576,35 @@
         <v>100</v>
       </c>
       <c r="C20" s="1" t="n">
-        <f aca="false">SUM(C21:C29)</f>
+        <f aca="false">SUM(C21:C30)</f>
         <v>256</v>
       </c>
       <c r="D20" s="1" t="n">
-        <f aca="false">SUM(D21:D29)</f>
+        <f aca="false">SUM(D21:D30)</f>
         <v>202</v>
       </c>
       <c r="E20" s="1" t="n">
-        <f aca="false">SUM(E21:E29)</f>
-        <v>127</v>
+        <f aca="false">SUM(E21:E30)</f>
+        <v>129</v>
       </c>
       <c r="F20" s="1" t="n">
-        <f aca="false">SUM(F21:F29)</f>
+        <f aca="false">SUM(F21:F30)</f>
         <v>105</v>
       </c>
       <c r="G20" s="1" t="n">
-        <f aca="false">SUM(G21:G29)</f>
+        <f aca="false">SUM(G21:G30)</f>
         <v>82</v>
       </c>
       <c r="H20" s="1" t="n">
-        <f aca="false">SUM(H21:H29)</f>
+        <f aca="false">SUM(H21:H30)</f>
         <v>133</v>
       </c>
       <c r="I20" s="1" t="n">
-        <f aca="false">SUM(I21:I29)</f>
+        <f aca="false">SUM(I21:I30)</f>
         <v>43</v>
       </c>
       <c r="J20" s="1" t="n">
-        <f aca="false">SUM(J21:J29)</f>
+        <f aca="false">SUM(J21:J30)</f>
         <v>25</v>
       </c>
     </row>
@@ -3749,987 +3746,987 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="30" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <f aca="false">SUM(C31:C39)</f>
-        <v>34</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <f aca="false">SUM(D31:D39)</f>
-        <v>76</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <f aca="false">SUM(E31:E39)</f>
-        <v>7</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <f aca="false">SUM(F31:F39)</f>
+      <c r="C31" s="1" t="n">
+        <f aca="false">SUM(C32:C45)</f>
+        <v>99</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">SUM(D32:D45)</f>
+        <v>127</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">SUM(E32:E45)</f>
+        <v>9</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">SUM(F32:F45)</f>
+        <v>8</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <f aca="false">SUM(G32:G45)</f>
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <f aca="false">SUM(H32:H45)</f>
+        <v>66</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <f aca="false">SUM(I32:I45)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="1" t="n">
-        <f aca="false">SUM(G31:G39)</f>
-        <v>12</v>
-      </c>
-      <c r="H30" s="1" t="n">
-        <f aca="false">SUM(H31:H39)</f>
-        <v>35</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <f aca="false">SUM(I31:I39)</f>
+      <c r="J31" s="1" t="n">
+        <f aca="false">SUM(J32:J45)</f>
         <v>0</v>
-      </c>
-      <c r="J30" s="1" t="n">
-        <f aca="false">SUM(J31:J39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="D31" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="H31" s="4" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="32" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C32" s="4" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>45</v>
-      </c>
-      <c r="E32" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G32" s="4" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C34" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E34" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="4" t="s">
-        <v>88</v>
+        <v>54</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>1</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="4" t="n">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H36" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="4" t="s">
-        <v>83</v>
+        <v>45</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="D37" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="38" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H38" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <f aca="false">SUM(C41:C45)</f>
-        <v>42</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <f aca="false">SUM(D41:D45)</f>
-        <v>29</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <f aca="false">SUM(E41:E45)</f>
-        <v>1</v>
-      </c>
-      <c r="F40" s="1" t="n">
-        <f aca="false">SUM(F41:F45)</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <f aca="false">SUM(G41:G45)</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="1" t="n">
-        <f aca="false">SUM(H41:H45)</f>
-        <v>16</v>
-      </c>
-      <c r="I40" s="1" t="n">
-        <f aca="false">SUM(I41:I45)</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="1" t="n">
-        <f aca="false">SUM(J41:J45)</f>
-        <v>0</v>
+      <c r="D40" s="4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D41" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="E41" s="4" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C42" s="4" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D42" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="H42" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C43" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="F43" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="D43" s="4" t="n">
-        <v>11</v>
-      </c>
       <c r="H43" s="4" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
+      </c>
+      <c r="C44" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="D44" s="4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="4" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C45" s="4" t="n">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E45" s="4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="n">
-        <f aca="false">SUM(C47:C48)</f>
-        <v>29</v>
+        <f aca="false">SUM(C47:C53)</f>
+        <v>42</v>
       </c>
       <c r="D46" s="1" t="n">
-        <f aca="false">SUM(D47:D48)</f>
-        <v>1</v>
+        <f aca="false">SUM(D47:D53)</f>
+        <v>49</v>
       </c>
       <c r="E46" s="1" t="n">
-        <f aca="false">SUM(E47:E48)</f>
+        <f aca="false">SUM(E47:E53)</f>
+        <v>1</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <f aca="false">SUM(F47:F53)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="1" t="n">
-        <f aca="false">SUM(F47:F48)</f>
+      <c r="G46" s="1" t="n">
+        <f aca="false">SUM(G47:G53)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="1" t="n">
-        <f aca="false">SUM(G47:G48)</f>
+      <c r="H46" s="1" t="n">
+        <f aca="false">SUM(H47:H53)</f>
+        <v>16</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <f aca="false">SUM(I47:I53)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="1" t="n">
-        <f aca="false">SUM(H47:H48)</f>
-        <v>14</v>
-      </c>
-      <c r="I46" s="1" t="n">
-        <f aca="false">SUM(I47:I48)</f>
-        <v>0</v>
-      </c>
       <c r="J46" s="1" t="n">
-        <f aca="false">SUM(J47:J48)</f>
+        <f aca="false">SUM(J47:J53)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="H47" s="4" t="n">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D47" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E47" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C48" s="4" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D48" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <f aca="false">SUM(C50:C55)</f>
-        <v>64</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <f aca="false">SUM(D50:D55)</f>
-        <v>94</v>
-      </c>
-      <c r="E49" s="1" t="n">
-        <f aca="false">SUM(E50:E55)</f>
         <v>9</v>
       </c>
-      <c r="F49" s="1" t="n">
-        <f aca="false">SUM(F50:F55)</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <f aca="false">SUM(G50:G55)</f>
-        <v>27</v>
-      </c>
-      <c r="H49" s="1" t="n">
-        <f aca="false">SUM(H50:H55)</f>
-        <v>41</v>
-      </c>
-      <c r="I49" s="1" t="n">
-        <f aca="false">SUM(I50:I55)</f>
-        <v>0</v>
-      </c>
-      <c r="J49" s="1" t="n">
-        <f aca="false">SUM(J50:J55)</f>
-        <v>0</v>
+      <c r="H48" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="50" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="4" t="n">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="D50" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="E50" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G50" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H50" s="4" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C51" s="4" t="n">
-        <v>17</v>
-      </c>
-      <c r="D51" s="4" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" s="4" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="4" t="n">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="D53" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="G53" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="H53" s="4" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D54" s="4" t="n">
-        <v>17</v>
-      </c>
-      <c r="E54" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G54" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H54" s="4" t="n">
-        <v>11</v>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <f aca="false">SUM(C55:C57)</f>
+        <v>45</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <f aca="false">SUM(D55:D57)</f>
+        <v>1</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">SUM(E55:E57)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <f aca="false">SUM(F55:F57)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <f aca="false">SUM(G55:G57)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <f aca="false">SUM(H55:H57)</f>
+        <v>30</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <f aca="false">SUM(I55:I57)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <f aca="false">SUM(J55:J57)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="55" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="C55" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="D55" s="4" t="n">
-        <v>19</v>
-      </c>
-      <c r="G55" s="4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <f aca="false">SUM(C57:C63)</f>
-        <v>19</v>
-      </c>
-      <c r="D56" s="1" t="n">
-        <f aca="false">SUM(D57:D63)</f>
-        <v>35</v>
-      </c>
-      <c r="E56" s="1" t="n">
-        <f aca="false">SUM(E57:E63)</f>
-        <v>6</v>
-      </c>
-      <c r="F56" s="1" t="n">
-        <f aca="false">SUM(F57:F63)</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="1" t="n">
-        <f aca="false">SUM(G57:G63)</f>
-        <v>10</v>
-      </c>
-      <c r="H56" s="1" t="n">
-        <f aca="false">SUM(H57:H63)</f>
-        <v>16</v>
-      </c>
-      <c r="I56" s="1" t="n">
-        <f aca="false">SUM(I57:I63)</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="1" t="n">
-        <f aca="false">SUM(J57:J63)</f>
-        <v>0</v>
+      <c r="H55" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D56" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="D58" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="E58" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G58" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="H58" s="4" t="n">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="C57" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <f aca="false">SUM(C59:C72)</f>
+        <v>64</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <f aca="false">SUM(D59:D72)</f>
+        <v>113</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <f aca="false">SUM(E59:E72)</f>
+        <v>9</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <f aca="false">SUM(F59:F72)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <f aca="false">SUM(G59:G72)</f>
+        <v>27</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <f aca="false">SUM(H59:H72)</f>
+        <v>41</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <f aca="false">SUM(I59:I72)</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <f aca="false">SUM(J59:J72)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="4" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C59" s="4" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D59" s="4" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E59" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="G59" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="H59" s="4" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="4" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C60" s="4" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D60" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H60" s="4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G61" s="4" t="n">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="D61" s="4" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="62" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="4" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="C62" s="4" t="n">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D62" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="G62" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="H62" s="4" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="63" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="4" t="s">
-        <v>69</v>
+        <v>44</v>
+      </c>
+      <c r="C63" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="D63" s="4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <f aca="false">SUM(C65:C71)</f>
-        <v>136</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <f aca="false">SUM(D65:D71)</f>
-        <v>213</v>
-      </c>
-      <c r="E64" s="1" t="n">
-        <f aca="false">SUM(E65:E71)</f>
-        <v>8</v>
-      </c>
-      <c r="F64" s="1" t="n">
-        <f aca="false">SUM(F65:F71)</f>
-        <v>0</v>
-      </c>
-      <c r="G64" s="1" t="n">
-        <f aca="false">SUM(G65:G71)</f>
-        <v>39</v>
-      </c>
-      <c r="H64" s="1" t="n">
-        <f aca="false">SUM(H65:H71)</f>
-        <v>76</v>
-      </c>
-      <c r="I64" s="1" t="n">
-        <f aca="false">SUM(I65:I71)</f>
-        <v>11</v>
-      </c>
-      <c r="J64" s="1" t="n">
-        <f aca="false">SUM(J65:J71)</f>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E63" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G63" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="D64" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="G64" s="4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="65" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="4" t="n">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D65" s="4" t="n">
-        <v>93</v>
-      </c>
-      <c r="E65" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="G65" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H65" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="I65" s="4" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="4" t="n">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D66" s="4" t="n">
-        <v>85</v>
-      </c>
-      <c r="G66" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="H66" s="4" t="n">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C67" s="4" t="n">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D67" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="G67" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" s="4" t="n">
-        <v>8</v>
+        <v>81</v>
+      </c>
+      <c r="D68" s="4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="69" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69" s="4" t="n">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="D69" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G69" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H69" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="4" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="D70" s="4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <f aca="false">SUM(C74:C80)</f>
+        <v>19</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <f aca="false">SUM(D74:D80)</f>
+        <v>35</v>
+      </c>
+      <c r="E73" s="1" t="n">
+        <f aca="false">SUM(E74:E80)</f>
+        <v>6</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <f aca="false">SUM(F74:F80)</f>
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="n">
+        <f aca="false">SUM(G74:G80)</f>
+        <v>10</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <f aca="false">SUM(H74:H80)</f>
+        <v>16</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <f aca="false">SUM(I74:I80)</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="1" t="n">
+        <f aca="false">SUM(J74:J80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D75" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="E75" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D76" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D77" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3"/>
+      <c r="B78" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G78" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <f aca="false">SUM(C82:C103)</f>
+        <v>148</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <f aca="false">SUM(D82:D103)</f>
+        <v>281</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <f aca="false">SUM(E82:E103)</f>
+        <v>8</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <f aca="false">SUM(F82:F103)</f>
+        <v>2</v>
+      </c>
+      <c r="G81" s="1" t="n">
+        <f aca="false">SUM(G82:G103)</f>
+        <v>45</v>
+      </c>
+      <c r="H81" s="1" t="n">
+        <f aca="false">SUM(H82:H103)</f>
+        <v>76</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <f aca="false">SUM(I82:I103)</f>
+        <v>11</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <f aca="false">SUM(J82:J103)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="D82" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="E82" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G82" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H82" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I82" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D83" s="4" t="n">
+        <v>85</v>
+      </c>
+      <c r="G83" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="H83" s="4" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D84" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G84" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C86" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D86" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G86" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H86" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D71" s="4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
+      <c r="D88" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C72" s="1" t="n">
-        <f aca="false">SUM(C73:C103)</f>
-        <v>87</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <f aca="false">SUM(D73:D103)</f>
-        <v>124</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <f aca="false">SUM(E73:E103)</f>
-        <v>4</v>
-      </c>
-      <c r="F72" s="1" t="n">
-        <f aca="false">SUM(F73:F103)</f>
-        <v>9</v>
-      </c>
-      <c r="G72" s="1" t="n">
-        <f aca="false">SUM(G73:G103)</f>
-        <v>3</v>
-      </c>
-      <c r="H72" s="1" t="n">
-        <f aca="false">SUM(H73:H103)</f>
-        <v>47</v>
-      </c>
-      <c r="I72" s="1" t="n">
-        <f aca="false">SUM(I73:I103)</f>
+      <c r="C89" s="1" t="n">
+        <f aca="false">SUM(C90:C103)</f>
+        <v>6</v>
+      </c>
+      <c r="D89" s="1" t="n">
+        <f aca="false">SUM(D90:D103)</f>
+        <v>34</v>
+      </c>
+      <c r="E89" s="1" t="n">
+        <f aca="false">SUM(E90:E103)</f>
         <v>0</v>
       </c>
-      <c r="J72" s="1" t="n">
-        <f aca="false">SUM(J73:J103)</f>
+      <c r="F89" s="1" t="n">
+        <f aca="false">SUM(F90:F103)</f>
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="n">
+        <f aca="false">SUM(G90:G103)</f>
+        <v>3</v>
+      </c>
+      <c r="H89" s="1" t="n">
+        <f aca="false">SUM(H90:H103)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D74" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="D75" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="F75" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H75" s="1" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D77" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D78" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E78" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="H79" s="1" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D80" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D82" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D83" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D84" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D85" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D86" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D87" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D88" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D89" s="1" t="n">
-        <v>4</v>
+      <c r="I89" s="1" t="n">
+        <f aca="false">SUM(I90:I103)</f>
+        <v>0</v>
+      </c>
+      <c r="J89" s="1" t="n">
+        <f aca="false">SUM(J90:J103)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D90" s="1" t="n">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D99" s="1" t="n">
         <v>1</v>
@@ -4737,7 +4734,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D100" s="1" t="n">
         <v>1</v>
@@ -4745,10 +4742,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E101" s="1" t="n">
-        <v>2</v>
+        <v>94</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,7 +4767,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4783,15 +4780,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4828,138 +4825,138 @@
         <v>99</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>265</v>
+        <v>314</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>15</v>
+        <v>202</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>256</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>202</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>0</v>
@@ -4970,25 +4967,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
@@ -4999,25 +4996,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
@@ -5028,124 +5025,37 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>94</v>
+        <v>281</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>136</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>213</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>76</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>124</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>